<commit_message>
Show the data from the database to the user
</commit_message>
<xml_diff>
--- a/People.xlsx
+++ b/People.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Folder\C# Projects\The C# Academy\ExcelReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E665CADE-73F3-4721-AA14-C8B6E17A5807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49529EC-9660-4E6E-A1D9-1C5A8B1C2730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6200" yWindow="4040" windowWidth="19200" windowHeight="11170" xr2:uid="{AB9EF0BA-E9B1-40FA-9502-8DA26D193C32}"/>
+    <workbookView xWindow="1510" yWindow="4110" windowWidth="19200" windowHeight="11170" xr2:uid="{AB9EF0BA-E9B1-40FA-9502-8DA26D193C32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,18 +119,12 @@
     <t>Martinez</t>
   </si>
   <si>
-    <t>kaitlinkaiser@example.com</t>
-  </si>
-  <si>
     <t>Lori</t>
   </si>
   <si>
     <t>Todd</t>
   </si>
   <si>
-    <t>buchananmanuel@example.net</t>
-  </si>
-  <si>
     <t>elijah57@example.net</t>
   </si>
   <si>
@@ -150,6 +144,12 @@
   </si>
   <si>
     <t>conniecowan@example.com</t>
+  </si>
+  <si>
+    <t>kaitkaiser@example.com</t>
+  </si>
+  <si>
+    <t>bachmanuel@example.net</t>
   </si>
 </sst>
 </file>
@@ -516,7 +516,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -569,7 +569,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F2">
         <v>4084906784</v>
@@ -647,7 +647,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F5">
         <v>7840946111</v>
@@ -664,16 +664,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F6">
         <v>6892073558</v>
@@ -690,16 +690,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F7">
         <v>3716499856</v>
@@ -716,16 +716,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F8">
         <v>7731516685</v>

</xml_diff>

<commit_message>
Add the functionality to write more data to the excel file
</commit_message>
<xml_diff>
--- a/People.xlsx
+++ b/People.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Folder\C# Projects\The C# Academy\ExcelReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49529EC-9660-4E6E-A1D9-1C5A8B1C2730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5227640A-8DAD-4B15-AB73-040BF4C8A67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1510" yWindow="4110" windowWidth="19200" windowHeight="11170" xr2:uid="{AB9EF0BA-E9B1-40FA-9502-8DA26D193C32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Index</t>
   </si>
@@ -71,6 +71,9 @@
     <t>Male</t>
   </si>
   <si>
+    <t>elijah57@example.net</t>
+  </si>
+  <si>
     <t>Games developer</t>
   </si>
   <si>
@@ -86,6 +89,9 @@
     <t>bethany14@example.com</t>
   </si>
   <si>
+    <t>Phytotherapist</t>
+  </si>
+  <si>
     <t>Kristine</t>
   </si>
   <si>
@@ -95,68 +101,99 @@
     <t>bthompson@example.com</t>
   </si>
   <si>
-    <t>Phytotherapist</t>
-  </si>
-  <si>
     <t>Homeopath</t>
   </si>
   <si>
+    <t>Yesenia</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>kaitkaiser@example.com</t>
+  </si>
+  <si>
     <t>Market researcher</t>
   </si>
   <si>
+    <t>Lori</t>
+  </si>
+  <si>
+    <t>Todd</t>
+  </si>
+  <si>
+    <t>bachmanuel@example.net</t>
+  </si>
+  <si>
     <t>Veterinary surgeon</t>
   </si>
   <si>
+    <t>Erin</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>tconner@example.org</t>
+  </si>
+  <si>
     <t>Waste management officer</t>
   </si>
   <si>
+    <t>Katherine</t>
+  </si>
+  <si>
+    <t>Buck</t>
+  </si>
+  <si>
+    <t>conniecowan@example.com</t>
+  </si>
+  <si>
     <t>Intelligence analyst</t>
   </si>
   <si>
-    <t>Yesenia</t>
-  </si>
-  <si>
-    <t>Martinez</t>
-  </si>
-  <si>
-    <t>Lori</t>
-  </si>
-  <si>
-    <t>Todd</t>
-  </si>
-  <si>
-    <t>elijah57@example.net</t>
-  </si>
-  <si>
-    <t>Erin</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>tconner@example.org</t>
-  </si>
-  <si>
-    <t>Katherine</t>
-  </si>
-  <si>
-    <t>Buck</t>
-  </si>
-  <si>
-    <t>conniecowan@example.com</t>
-  </si>
-  <si>
-    <t>kaitkaiser@example.com</t>
-  </si>
-  <si>
-    <t>bachmanuel@example.net</t>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>johnsmith@example.com</t>
+  </si>
+  <si>
+    <t>5378512935</t>
+  </si>
+  <si>
+    <t>05-Feb-98</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>emilyjackson@example.net</t>
+  </si>
+  <si>
+    <t>7325418495</t>
+  </si>
+  <si>
+    <t>21-Jul-97</t>
+  </si>
+  <si>
+    <t>Psychiatrist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,12 +229,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="1" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -513,241 +550,296 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22305F2-A4BC-44F6-A7A1-24A4748A5B4C}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="24.897998809814453" customWidth="1"/>
+    <col min="6" max="6" bestFit="1" width="11.634980201721191" customWidth="1"/>
+    <col min="7" max="7" bestFit="1" width="9.593964576721191" customWidth="1"/>
+    <col min="8" max="8" bestFit="1" width="10.746960639953613" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2">
+        <v>11</v>
+      </c>
+      <c r="F2" s="0">
         <v>4084906784</v>
       </c>
       <c r="G2" s="2">
         <v>24041</v>
       </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="H2" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3">
+        <v>16</v>
+      </c>
+      <c r="F3" s="0">
         <v>6141126044</v>
       </c>
       <c r="G3" s="2">
         <v>25651</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="F4" s="0">
         <v>8776097938</v>
       </c>
       <c r="G4" s="2">
         <v>33787</v>
       </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="H4" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5">
+        <v>24</v>
+      </c>
+      <c r="F5" s="0">
         <v>7840946111</v>
       </c>
       <c r="G5" s="2">
         <v>35645</v>
       </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="H5" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>6892073558</v>
       </c>
       <c r="G6" s="2">
         <v>32478</v>
       </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="H6" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>3716499856</v>
       </c>
       <c r="G7" s="2">
         <v>35000</v>
       </c>
-      <c r="H7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="H7" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
-        <v>14</v>
+      <c r="C8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8">
+        <v>36</v>
+      </c>
+      <c r="F8" s="0">
         <v>7731516685</v>
       </c>
       <c r="G8" s="2">
         <v>32530</v>
       </c>
-      <c r="H8" t="s">
-        <v>24</v>
+      <c r="H8" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>73</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>81</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{3ECE1999-0F8F-4A35-88D2-1DE9570FB792}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{07E3B55A-0E1F-46BC-AB92-2650FABA12E4}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{5F19C91A-5A46-42AD-BE56-0E3E74E6AEAA}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{23B6406E-9AF1-4D89-ADD0-E7932FA857D7}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{F0513F36-F2C5-4662-9B9E-430AA6EF0CC6}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{0E2856A3-B1FD-4F36-A59A-149C027FEDBA}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{4BB1EE87-DF9B-4F14-9B53-9B22079E8CA5}"/>
+    <hyperlink ref="E2" r:id="rId7"/>
+    <hyperlink ref="E3" r:id="rId8"/>
+    <hyperlink ref="E4" r:id="rId9"/>
+    <hyperlink ref="E5" r:id="rId10"/>
+    <hyperlink ref="E6" r:id="rId11"/>
+    <hyperlink ref="E7" r:id="rId12"/>
+    <hyperlink ref="E8" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>